<commit_message>
Create Try-Catch for member search failures
</commit_message>
<xml_diff>
--- a/Error Codes.xlsx
+++ b/Error Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evils\Documents\UiPath\MedicalReadinessDiscrepancies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BC6354-983F-45BA-877C-7EB0D4FFE2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A99733B-EBD6-48C5-A3FC-B7F59E994F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Error Code</t>
   </si>
   <si>
     <t>Amplifying Information</t>
+  </si>
+  <si>
+    <t>NO_MATCHING_RECORD</t>
+  </si>
+  <si>
+    <t>No match found in MRRS Report. Sailor may not be locally gained in MRRS.</t>
   </si>
 </sst>
 </file>
@@ -348,16 +354,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -368,6 +374,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated flu processing to utilize error code datatable
</commit_message>
<xml_diff>
--- a/Error Codes.xlsx
+++ b/Error Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evils\Documents\UiPath\MedicalReadinessDiscrepancies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A99733B-EBD6-48C5-A3FC-B7F59E994F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7B9B84-70C6-4EA4-8014-BB655845CD86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Error Code</t>
   </si>
@@ -37,6 +37,33 @@
   </si>
   <si>
     <t>No match found in MRRS Report. Sailor may not be locally gained in MRRS.</t>
+  </si>
+  <si>
+    <t>Multiple matches found in MRRS Report. Sailor's info will have to be checked manually.</t>
+  </si>
+  <si>
+    <t>MULTIPLE_RECORDS_FOUND</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Record Search</t>
+  </si>
+  <si>
+    <t>INFLUENZA_OVERDUE</t>
+  </si>
+  <si>
+    <t>Influenza out of date in MRRS. Verify with physical record and MHS Genesis.</t>
+  </si>
+  <si>
+    <t>Influeza Verification</t>
+  </si>
+  <si>
+    <t>NO_DOCUMENTED_INFLUENZA</t>
+  </si>
+  <si>
+    <t>No documented influenza in MRRS. Verify with physical record and MHS Genesis.</t>
   </si>
 </sst>
 </file>
@@ -354,32 +381,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test to check for proper error code
</commit_message>
<xml_diff>
--- a/Error Codes.xlsx
+++ b/Error Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evils\Documents\UiPath\MedicalReadinessDiscrepancies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7B9B84-70C6-4EA4-8014-BB655845CD86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA03FB2-BC3F-4197-BA0D-BC60EADE88A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Error Code</t>
   </si>
@@ -64,6 +64,21 @@
   </si>
   <si>
     <t>No documented influenza in MRRS. Verify with physical record and MHS Genesis.</t>
+  </si>
+  <si>
+    <t>NO_BLOOD_TYPE_DATE</t>
+  </si>
+  <si>
+    <t>NO_BLOOD_TYPE_RESULT</t>
+  </si>
+  <si>
+    <t>No documented blood type result. Verify in patient's physical record and Genesis.</t>
+  </si>
+  <si>
+    <t>Blood Type Verification</t>
+  </si>
+  <si>
+    <t>No documented blood type date (G6PD Date). Verify in patient's physical record and Genesis.</t>
   </si>
 </sst>
 </file>
@@ -381,17 +396,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -449,6 +464,28 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>